<commit_message>
koksag prime number after 19
why am i wasting time on this instead of rainworld
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -257,12 +257,6 @@
   </si>
   <si>
     <t>M4A1/AR15</t>
-  </si>
-  <si>
-    <t>SG556/2/whatever</t>
-  </si>
-  <si>
-    <t>G18/G20</t>
   </si>
   <si>
     <t>MAC10/11</t>
@@ -339,6 +333,12 @@
       <t xml:space="preserve"> =  unofficial (be it from other mod or stolen from god knows where)</t>
     </r>
   </si>
+  <si>
+    <t>G17/18/19/20</t>
+  </si>
+  <si>
+    <t>SG552/3/6/whatever</t>
+  </si>
 </sst>
 </file>
 
@@ -904,24 +904,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -940,31 +958,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,12 +1947,12 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
       <c r="G24" s="21"/>
@@ -1960,13 +1960,13 @@
       <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="A25" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
@@ -1985,69 +1985,69 @@
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29" t="s">
+      <c r="A28" s="25"/>
+      <c r="B28" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29" t="s">
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H28" s="29" t="s">
+      <c r="H28" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="I28" s="30" t="s">
+      <c r="I28" s="27" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="33"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="34"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="36"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="42"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
+      <c r="A31" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="27" t="s">
+      <c r="F31" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
       <c r="I31" s="46"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="39"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="22">
         <v>3</v>
       </c>
@@ -2057,10 +2057,10 @@
       <c r="D32" s="24">
         <v>2</v>
       </c>
-      <c r="E32" s="41" t="s">
+      <c r="E32" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="44"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="22">
         <v>11</v>
       </c>
@@ -2072,7 +2072,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="6" t="s">
         <v>78</v>
       </c>
@@ -2082,10 +2082,10 @@
       <c r="D33" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="41" t="s">
+      <c r="E33" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="44"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="6">
         <v>13</v>
       </c>
@@ -2097,32 +2097,32 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="39"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="6">
         <v>2</v>
       </c>
       <c r="C34" s="2">
         <v>2</v>
       </c>
-      <c r="D34" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="41" t="s">
+      <c r="D34" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="44"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="6">
         <v>4</v>
       </c>
       <c r="H34" s="2">
         <v>5</v>
       </c>
-      <c r="I34" s="37" t="s">
+      <c r="I34" s="28" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="6">
         <v>3</v>
       </c>
@@ -2132,10 +2132,10 @@
       <c r="D35" s="7">
         <v>2</v>
       </c>
-      <c r="E35" s="41" t="s">
+      <c r="E35" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="44"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="6">
         <v>10</v>
       </c>
@@ -2147,7 +2147,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="39"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="6">
         <v>2</v>
       </c>
@@ -2157,10 +2157,10 @@
       <c r="D36" s="7">
         <v>0</v>
       </c>
-      <c r="E36" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" s="44"/>
+      <c r="E36" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" s="34"/>
       <c r="G36" s="6">
         <v>8</v>
       </c>
@@ -2172,7 +2172,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="39"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="6">
         <v>3</v>
       </c>
@@ -2182,10 +2182,10 @@
       <c r="D37" s="7">
         <v>2</v>
       </c>
-      <c r="E37" s="41" t="s">
+      <c r="E37" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="F37" s="44"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="6">
         <v>8</v>
       </c>
@@ -2197,7 +2197,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="39"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="6">
         <v>3</v>
       </c>
@@ -2207,10 +2207,10 @@
       <c r="D38" s="7">
         <v>2</v>
       </c>
-      <c r="E38" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" s="44"/>
+      <c r="E38" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="34"/>
       <c r="G38" s="6">
         <v>7</v>
       </c>
@@ -2222,35 +2222,35 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="39"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="6">
         <v>3</v>
       </c>
-      <c r="C39" s="38">
+      <c r="C39" s="29">
         <v>5</v>
       </c>
       <c r="D39" s="7">
         <v>0</v>
       </c>
-      <c r="E39" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="F39" s="44"/>
+      <c r="E39" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="F39" s="34"/>
       <c r="G39" s="6">
         <v>8</v>
       </c>
-      <c r="H39" s="38">
+      <c r="H39" s="29">
         <v>3</v>
       </c>
       <c r="I39" s="7">
         <v>2</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="40"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="8">
         <v>2</v>
       </c>
@@ -2260,10 +2260,10 @@
       <c r="D40" s="10">
         <v>0</v>
       </c>
-      <c r="E40" s="42" t="s">
+      <c r="E40" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="45"/>
+      <c r="F40" s="35"/>
       <c r="G40" s="8">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
mac11 pdw stock, m4 sliding stock
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -1274,7 +1274,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:E25"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1327,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>62</v>
@@ -1566,7 +1566,7 @@
         <v>3</v>
       </c>
       <c r="I9" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>62</v>
@@ -2215,7 +2215,7 @@
         <v>3</v>
       </c>
       <c r="I38" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fuck am i doing
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -1273,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,7 +1417,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>

</xml_diff>

<commit_message>
reload logic, quad barrel
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -215,9 +215,6 @@
   </si>
   <si>
     <t>do I have to ?</t>
-  </si>
-  <si>
-    <t>h</t>
   </si>
   <si>
     <t>one off gun is fun</t>
@@ -335,6 +332,9 @@
   </si>
   <si>
     <t>Need: more pistol stock*, more lhik option,  wire stock</t>
+  </si>
+  <si>
+    <t>its gonna b smth I guess</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1274,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,7 +1490,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>30</v>
@@ -1522,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>31</v>
@@ -1554,7 +1554,7 @@
         <v>39</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>32</v>
@@ -1586,7 +1586,7 @@
         <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>33</v>
@@ -1682,7 +1682,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>37</v>
@@ -1697,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1729,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1746,7 +1746,7 @@
         <v>39</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>19</v>
@@ -1857,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1906,7 +1906,7 @@
         <v>40</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1945,7 +1945,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
@@ -1987,7 +1987,7 @@
         <v>38</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>1</v>
@@ -1998,7 +1998,7 @@
         <v>38</v>
       </c>
       <c r="H28" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I28" s="27" t="s">
         <v>1</v>
@@ -2006,7 +2006,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="38"/>
       <c r="C29" s="38"/>
@@ -2030,14 +2030,14 @@
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
       <c r="D31" s="44"/>
       <c r="E31" s="4"/>
       <c r="F31" s="45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G31" s="44"/>
       <c r="H31" s="44"/>
@@ -2071,16 +2071,16 @@
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C33" s="2">
         <v>6</v>
       </c>
       <c r="D33" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="32" t="s">
         <v>77</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>78</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="6">
@@ -2155,7 +2155,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="6">
@@ -2205,7 +2205,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="6">
@@ -2230,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F39" s="34"/>
       <c r="G39" s="6">
@@ -2243,7 +2243,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>